<commit_message>
Some error code handling.
</commit_message>
<xml_diff>
--- a/Design Docs/Possible Actions.xlsx
+++ b/Design Docs/Possible Actions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>Engines</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Hatch</t>
   </si>
   <si>
-    <t>Restraints</t>
-  </si>
-  <si>
     <t>Open</t>
   </si>
   <si>
@@ -97,6 +94,39 @@
   </si>
   <si>
     <t>Personnell Supports</t>
+  </si>
+  <si>
+    <t>Restraints On</t>
+  </si>
+  <si>
+    <t>Restraints Off</t>
+  </si>
+  <si>
+    <t>Error Codes</t>
+  </si>
+  <si>
+    <t>E1908</t>
+  </si>
+  <si>
+    <t>Invalid Verb</t>
+  </si>
+  <si>
+    <t>E1976</t>
+  </si>
+  <si>
+    <t>Invalid Noun</t>
+  </si>
+  <si>
+    <t>E7702</t>
+  </si>
+  <si>
+    <t>O2 System Not On</t>
+  </si>
+  <si>
+    <t>E7856</t>
+  </si>
+  <si>
+    <t>CO2 Scrubber Not On</t>
   </si>
 </sst>
 </file>
@@ -429,15 +459,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -470,7 +501,7 @@
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
       <c r="D3" t="s">
@@ -526,7 +557,7 @@
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -646,13 +677,13 @@
         <v>88</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20">
         <v>77</v>
       </c>
       <c r="D20" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -660,33 +691,81 @@
         <v>88</v>
       </c>
       <c r="D21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="C22">
+        <v>99</v>
+      </c>
+      <c r="D22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
-      <c r="A22">
+    <row r="23" spans="1:4">
+      <c r="A23">
         <v>99</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>21</v>
       </c>
-      <c r="C22">
+      <c r="C23">
         <v>44</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="C24">
+        <v>56</v>
+      </c>
+      <c r="D24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
-      <c r="C23">
-        <v>56</v>
-      </c>
-      <c r="D23" t="s">
-        <v>24</v>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="C3" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>